<commit_message>
Updated side data, various fixes for more accurate import
</commit_message>
<xml_diff>
--- a/tabular/Troupin-data.xlsx
+++ b/tabular/Troupin-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="892">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -2690,6 +2690,12 @@
   </si>
   <si>
     <t>Liu et al. unpublished</t>
+  </si>
+  <si>
+    <t>Complete genome</t>
+  </si>
+  <si>
+    <t>Coverage</t>
   </si>
 </sst>
 </file>
@@ -2759,8 +2765,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2943,7 +2953,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3028,6 +3038,8 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3112,6 +3124,8 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3441,10 +3455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I319"/>
+  <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3458,9 +3472,10 @@
     <col min="7" max="7" width="33.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="31" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>872</v>
       </c>
@@ -3488,8 +3503,11 @@
       <c r="I1" s="1" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>657</v>
       </c>
@@ -3517,8 +3535,11 @@
       <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>667</v>
       </c>
@@ -3546,8 +3567,11 @@
       <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>668</v>
       </c>
@@ -3575,8 +3599,11 @@
       <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>674</v>
       </c>
@@ -3604,8 +3631,11 @@
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>675</v>
       </c>
@@ -3633,8 +3663,11 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -3662,8 +3695,11 @@
       <c r="I7" s="2">
         <v>-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>677</v>
       </c>
@@ -3691,8 +3727,11 @@
       <c r="I8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>678</v>
       </c>
@@ -3720,8 +3759,11 @@
       <c r="I9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>705</v>
       </c>
@@ -3749,8 +3791,11 @@
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>732</v>
       </c>
@@ -3778,8 +3823,11 @@
       <c r="I11" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>733</v>
       </c>
@@ -3807,8 +3855,11 @@
       <c r="I12" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>734</v>
       </c>
@@ -3836,8 +3887,11 @@
       <c r="I13" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>743</v>
       </c>
@@ -3865,8 +3919,11 @@
       <c r="I14" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>744</v>
       </c>
@@ -3894,8 +3951,11 @@
       <c r="I15" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>761</v>
       </c>
@@ -3923,8 +3983,11 @@
       <c r="I16" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>762</v>
       </c>
@@ -3952,8 +4015,11 @@
       <c r="I17" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>361</v>
       </c>
@@ -3981,8 +4047,11 @@
       <c r="I18" s="2">
         <v>-23</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>791</v>
       </c>
@@ -4010,8 +4079,11 @@
       <c r="I19" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>792</v>
       </c>
@@ -4039,8 +4111,11 @@
       <c r="I20" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>660</v>
       </c>
@@ -4068,8 +4143,11 @@
       <c r="I21" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>661</v>
       </c>
@@ -4097,8 +4175,11 @@
       <c r="I22" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>801</v>
       </c>
@@ -4126,8 +4207,11 @@
       <c r="I23" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>802</v>
       </c>
@@ -4155,8 +4239,11 @@
       <c r="I24" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>803</v>
       </c>
@@ -4184,8 +4271,11 @@
       <c r="I25" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
         <v>804</v>
       </c>
@@ -4213,8 +4303,11 @@
       <c r="I26" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
         <v>704</v>
       </c>
@@ -4242,8 +4335,11 @@
       <c r="I27" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>400</v>
       </c>
@@ -4271,8 +4367,11 @@
       <c r="I28" s="2" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>815</v>
       </c>
@@ -4300,8 +4399,11 @@
       <c r="I29" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>816</v>
       </c>
@@ -4329,8 +4431,11 @@
       <c r="I30" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
         <v>230</v>
       </c>
@@ -4358,8 +4463,11 @@
       <c r="I31" s="2" t="s">
         <v>874</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>232</v>
       </c>
@@ -4387,8 +4495,11 @@
       <c r="I32" s="2">
         <v>-16</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
         <v>235</v>
       </c>
@@ -4416,8 +4527,11 @@
       <c r="I33" s="2" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
         <v>368</v>
       </c>
@@ -4445,8 +4559,11 @@
       <c r="I34" s="2" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
         <v>370</v>
       </c>
@@ -4474,8 +4591,11 @@
       <c r="I35" s="2" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
         <v>651</v>
       </c>
@@ -4503,8 +4623,11 @@
       <c r="I36" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
         <v>652</v>
       </c>
@@ -4532,8 +4655,11 @@
       <c r="I37" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="2" t="s">
         <v>653</v>
       </c>
@@ -4561,8 +4687,11 @@
       <c r="I38" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
         <v>126</v>
       </c>
@@ -4590,8 +4719,11 @@
       <c r="I39" s="2" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
         <v>449</v>
       </c>
@@ -4619,8 +4751,11 @@
       <c r="I40" s="2">
         <v>-25</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="2" t="s">
         <v>451</v>
       </c>
@@ -4648,8 +4783,11 @@
       <c r="I41" s="2">
         <v>-25</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="2" t="s">
         <v>453</v>
       </c>
@@ -4677,8 +4815,11 @@
       <c r="I42" s="2">
         <v>-25</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
         <v>760</v>
       </c>
@@ -4706,8 +4847,11 @@
       <c r="I43" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
         <v>680</v>
       </c>
@@ -4735,8 +4879,11 @@
       <c r="I44" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="2" t="s">
         <v>123</v>
       </c>
@@ -4764,8 +4911,11 @@
       <c r="I45" s="2">
         <v>-7</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
         <v>159</v>
       </c>
@@ -4793,8 +4943,11 @@
       <c r="I46" s="2">
         <v>-7</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="2" t="s">
         <v>713</v>
       </c>
@@ -4822,8 +4975,11 @@
       <c r="I47" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
         <v>681</v>
       </c>
@@ -4851,8 +5007,11 @@
       <c r="I48" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="2" t="s">
         <v>97</v>
       </c>
@@ -4880,8 +5039,11 @@
       <c r="I49" s="2">
         <v>-5</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
         <v>101</v>
       </c>
@@ -4909,8 +5071,11 @@
       <c r="I50" s="2">
         <v>-6</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="2" t="s">
         <v>104</v>
       </c>
@@ -4938,8 +5103,11 @@
       <c r="I51" s="2" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
         <v>108</v>
       </c>
@@ -4967,8 +5135,11 @@
       <c r="I52" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
         <v>110</v>
       </c>
@@ -4996,8 +5167,11 @@
       <c r="I53" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="2" t="s">
         <v>112</v>
       </c>
@@ -5025,8 +5199,11 @@
       <c r="I54" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
         <v>114</v>
       </c>
@@ -5054,8 +5231,11 @@
       <c r="I55" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="2" t="s">
         <v>116</v>
       </c>
@@ -5083,8 +5263,11 @@
       <c r="I56" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="2" t="s">
         <v>119</v>
       </c>
@@ -5112,8 +5295,11 @@
       <c r="I57" s="2" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="2" t="s">
         <v>121</v>
       </c>
@@ -5141,8 +5327,11 @@
       <c r="I58" s="2" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
         <v>128</v>
       </c>
@@ -5170,8 +5359,11 @@
       <c r="I59" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
         <v>130</v>
       </c>
@@ -5199,8 +5391,11 @@
       <c r="I60" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
         <v>138</v>
       </c>
@@ -5228,8 +5423,11 @@
       <c r="I61" s="2" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="2" t="s">
         <v>140</v>
       </c>
@@ -5257,8 +5455,11 @@
       <c r="I62" s="2" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="2" t="s">
         <v>142</v>
       </c>
@@ -5286,8 +5487,11 @@
       <c r="I63" s="2" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="2" t="s">
         <v>150</v>
       </c>
@@ -5315,8 +5519,11 @@
       <c r="I64" s="2">
         <v>-11</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
         <v>155</v>
       </c>
@@ -5344,8 +5551,11 @@
       <c r="I65" s="2">
         <v>-13</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
         <v>157</v>
       </c>
@@ -5373,8 +5583,11 @@
       <c r="I66" s="2" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="2" t="s">
         <v>161</v>
       </c>
@@ -5402,8 +5615,11 @@
       <c r="I67" s="2">
         <v>-7</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="2" t="s">
         <v>164</v>
       </c>
@@ -5431,8 +5647,11 @@
       <c r="I68" s="2">
         <v>-14</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
         <v>169</v>
       </c>
@@ -5460,8 +5679,11 @@
       <c r="I69" s="2">
         <v>-15</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
         <v>679</v>
       </c>
@@ -5489,8 +5711,11 @@
       <c r="I70" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="2" t="s">
         <v>106</v>
       </c>
@@ -5518,8 +5743,11 @@
       <c r="I71" s="2" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" s="2" t="s">
         <v>145</v>
       </c>
@@ -5547,8 +5775,11 @@
       <c r="I72" s="2">
         <v>-10</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="2" t="s">
         <v>147</v>
       </c>
@@ -5576,8 +5807,11 @@
       <c r="I73" s="2">
         <v>-7</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
         <v>152</v>
       </c>
@@ -5605,8 +5839,11 @@
       <c r="I74" s="2">
         <v>-12</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
         <v>95</v>
       </c>
@@ -5634,8 +5871,11 @@
       <c r="I75" s="2">
         <v>-5</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
         <v>99</v>
       </c>
@@ -5663,8 +5903,11 @@
       <c r="I76" s="2" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" s="2" t="s">
         <v>134</v>
       </c>
@@ -5692,8 +5935,11 @@
       <c r="I77" s="2">
         <v>-9</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" s="2" t="s">
         <v>136</v>
       </c>
@@ -5721,8 +5967,11 @@
       <c r="I78" s="2" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" s="2" t="s">
         <v>669</v>
       </c>
@@ -5750,8 +5999,11 @@
       <c r="I79" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" s="2" t="s">
         <v>670</v>
       </c>
@@ -5779,8 +6031,11 @@
       <c r="I80" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="2" t="s">
         <v>671</v>
       </c>
@@ -5808,8 +6063,11 @@
       <c r="I81" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
         <v>672</v>
       </c>
@@ -5837,8 +6095,11 @@
       <c r="I82" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
         <v>673</v>
       </c>
@@ -5866,8 +6127,11 @@
       <c r="I83" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="2" t="s">
         <v>132</v>
       </c>
@@ -5895,8 +6159,11 @@
       <c r="I84" s="2">
         <v>-8</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="2" t="s">
         <v>736</v>
       </c>
@@ -5924,8 +6191,11 @@
       <c r="I85" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="2" t="s">
         <v>737</v>
       </c>
@@ -5953,8 +6223,11 @@
       <c r="I86" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="2" t="s">
         <v>738</v>
       </c>
@@ -5982,8 +6255,11 @@
       <c r="I87" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="2" t="s">
         <v>739</v>
       </c>
@@ -6011,8 +6287,11 @@
       <c r="I88" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="2" t="s">
         <v>281</v>
       </c>
@@ -6040,8 +6319,11 @@
       <c r="I89" s="2">
         <v>-18</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="2" t="s">
         <v>283</v>
       </c>
@@ -6069,8 +6351,11 @@
       <c r="I90" s="2">
         <v>-18</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="2" t="s">
         <v>755</v>
       </c>
@@ -6098,8 +6383,11 @@
       <c r="I91" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" s="2" t="s">
         <v>756</v>
       </c>
@@ -6127,8 +6415,11 @@
       <c r="I92" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" s="2" t="s">
         <v>475</v>
       </c>
@@ -6156,8 +6447,11 @@
       <c r="I93" s="2">
         <v>-28</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="2" t="s">
         <v>477</v>
       </c>
@@ -6185,8 +6479,11 @@
       <c r="I94" s="2">
         <v>-29</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" s="2" t="s">
         <v>770</v>
       </c>
@@ -6214,8 +6511,11 @@
       <c r="I95" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" s="2" t="s">
         <v>766</v>
       </c>
@@ -6243,8 +6543,11 @@
       <c r="I96" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" s="2" t="s">
         <v>767</v>
       </c>
@@ -6272,8 +6575,11 @@
       <c r="I97" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="2" t="s">
         <v>768</v>
       </c>
@@ -6301,8 +6607,11 @@
       <c r="I98" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="2" t="s">
         <v>769</v>
       </c>
@@ -6330,8 +6639,11 @@
       <c r="I99" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="J99" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="2" t="s">
         <v>770</v>
       </c>
@@ -6359,8 +6671,11 @@
       <c r="I100" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="J100" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="2" t="s">
         <v>463</v>
       </c>
@@ -6388,8 +6703,11 @@
       <c r="I101" s="2">
         <v>-27</v>
       </c>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="J101" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="2" t="s">
         <v>465</v>
       </c>
@@ -6417,8 +6735,11 @@
       <c r="I102" s="2">
         <v>-27</v>
       </c>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="J102" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" s="2" t="s">
         <v>467</v>
       </c>
@@ -6446,8 +6767,11 @@
       <c r="I103" s="2">
         <v>-27</v>
       </c>
-    </row>
-    <row r="104" spans="1:9">
+      <c r="J103" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="2" t="s">
         <v>663</v>
       </c>
@@ -6475,8 +6799,11 @@
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="J104" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" s="2" t="s">
         <v>45</v>
       </c>
@@ -6504,8 +6831,11 @@
       <c r="I105" s="2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="J105" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" s="2" t="s">
         <v>47</v>
       </c>
@@ -6533,8 +6863,11 @@
       <c r="I106" s="2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107" s="2" t="s">
         <v>696</v>
       </c>
@@ -6562,8 +6895,11 @@
       <c r="I107" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="J107" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108" s="2" t="s">
         <v>697</v>
       </c>
@@ -6591,8 +6927,11 @@
       <c r="I108" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="J108" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109" s="2" t="s">
         <v>655</v>
       </c>
@@ -6620,8 +6959,11 @@
       <c r="I109" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="J109" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110" s="2" t="s">
         <v>528</v>
       </c>
@@ -6649,8 +6991,11 @@
       <c r="I110" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="J110" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111" s="2" t="s">
         <v>300</v>
       </c>
@@ -6678,8 +7023,11 @@
       <c r="I111" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="J111" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" s="2" t="s">
         <v>553</v>
       </c>
@@ -6707,8 +7055,11 @@
       <c r="I112" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" s="2" t="s">
         <v>642</v>
       </c>
@@ -6736,8 +7087,11 @@
       <c r="I113" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" s="2" t="s">
         <v>499</v>
       </c>
@@ -6765,8 +7119,11 @@
       <c r="I114" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="2" t="s">
         <v>506</v>
       </c>
@@ -6794,8 +7151,11 @@
       <c r="I115" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116" s="2" t="s">
         <v>508</v>
       </c>
@@ -6823,8 +7183,11 @@
       <c r="I116" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" s="2" t="s">
         <v>525</v>
       </c>
@@ -6852,8 +7215,11 @@
       <c r="I117" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="J117" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118" s="2" t="s">
         <v>535</v>
       </c>
@@ -6881,8 +7247,11 @@
       <c r="I118" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="J118" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" s="2" t="s">
         <v>538</v>
       </c>
@@ -6910,8 +7279,11 @@
       <c r="I119" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="J119" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" s="2" t="s">
         <v>542</v>
       </c>
@@ -6939,8 +7311,11 @@
       <c r="I120" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="J120" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" s="2" t="s">
         <v>549</v>
       </c>
@@ -6968,8 +7343,11 @@
       <c r="I121" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="J121" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" s="2" t="s">
         <v>584</v>
       </c>
@@ -6997,8 +7375,11 @@
       <c r="I122" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="J122" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" s="2" t="s">
         <v>586</v>
       </c>
@@ -7026,8 +7407,11 @@
       <c r="I123" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="J123" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="2" t="s">
         <v>588</v>
       </c>
@@ -7055,8 +7439,11 @@
       <c r="I124" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="J124" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" s="2" t="s">
         <v>590</v>
       </c>
@@ -7084,8 +7471,11 @@
       <c r="I125" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="J125" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126" s="2" t="s">
         <v>592</v>
       </c>
@@ -7113,8 +7503,11 @@
       <c r="I126" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="J126" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" s="2" t="s">
         <v>594</v>
       </c>
@@ -7142,8 +7535,11 @@
       <c r="I127" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="128" spans="1:9">
+      <c r="J127" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128" s="2" t="s">
         <v>596</v>
       </c>
@@ -7171,8 +7567,11 @@
       <c r="I128" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="J128" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129" s="2" t="s">
         <v>598</v>
       </c>
@@ -7200,8 +7599,11 @@
       <c r="I129" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="130" spans="1:9">
+      <c r="J129" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130" s="2" t="s">
         <v>600</v>
       </c>
@@ -7229,8 +7631,11 @@
       <c r="I130" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="131" spans="1:9">
+      <c r="J130" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131" s="2" t="s">
         <v>602</v>
       </c>
@@ -7258,8 +7663,11 @@
       <c r="I131" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="132" spans="1:9">
+      <c r="J131" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132" s="2" t="s">
         <v>604</v>
       </c>
@@ -7287,8 +7695,11 @@
       <c r="I132" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="133" spans="1:9">
+      <c r="J132" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133" s="2" t="s">
         <v>606</v>
       </c>
@@ -7316,8 +7727,11 @@
       <c r="I133" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="134" spans="1:9">
+      <c r="J133" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134" s="2" t="s">
         <v>608</v>
       </c>
@@ -7345,8 +7759,11 @@
       <c r="I134" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="135" spans="1:9">
+      <c r="J134" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135" s="2" t="s">
         <v>610</v>
       </c>
@@ -7374,8 +7791,11 @@
       <c r="I135" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="136" spans="1:9">
+      <c r="J135" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136" s="2" t="s">
         <v>612</v>
       </c>
@@ -7403,8 +7823,11 @@
       <c r="I136" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="137" spans="1:9">
+      <c r="J136" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
       <c r="A137" s="2" t="s">
         <v>614</v>
       </c>
@@ -7432,8 +7855,11 @@
       <c r="I137" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="J137" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
       <c r="A138" s="2" t="s">
         <v>616</v>
       </c>
@@ -7461,8 +7887,11 @@
       <c r="I138" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="139" spans="1:9">
+      <c r="J138" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
       <c r="A139" s="2" t="s">
         <v>618</v>
       </c>
@@ -7490,8 +7919,11 @@
       <c r="I139" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="140" spans="1:9">
+      <c r="J139" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
       <c r="A140" s="2" t="s">
         <v>621</v>
       </c>
@@ -7519,8 +7951,11 @@
       <c r="I140" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="141" spans="1:9">
+      <c r="J140" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
       <c r="A141" s="2" t="s">
         <v>623</v>
       </c>
@@ -7548,8 +7983,11 @@
       <c r="I141" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="142" spans="1:9">
+      <c r="J141" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
       <c r="A142" s="2" t="s">
         <v>521</v>
       </c>
@@ -7577,8 +8015,11 @@
       <c r="I142" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="143" spans="1:9">
+      <c r="J142" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
       <c r="A143" s="2" t="s">
         <v>533</v>
       </c>
@@ -7606,8 +8047,11 @@
       <c r="I143" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="144" spans="1:9">
+      <c r="J143" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
       <c r="A144" s="2" t="s">
         <v>540</v>
       </c>
@@ -7635,8 +8079,11 @@
       <c r="I144" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="145" spans="1:9">
+      <c r="J144" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145" s="2" t="s">
         <v>573</v>
       </c>
@@ -7664,8 +8111,11 @@
       <c r="I145" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="146" spans="1:9">
+      <c r="J145" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146" s="2" t="s">
         <v>637</v>
       </c>
@@ -7693,8 +8143,11 @@
       <c r="I146" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="147" spans="1:9">
+      <c r="J146" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
       <c r="A147" s="2" t="s">
         <v>571</v>
       </c>
@@ -7722,8 +8175,11 @@
       <c r="I147" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="148" spans="1:9">
+      <c r="J147" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
       <c r="A148" s="2" t="s">
         <v>627</v>
       </c>
@@ -7751,8 +8207,11 @@
       <c r="I148" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="149" spans="1:9">
+      <c r="J148" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
       <c r="A149" s="2" t="s">
         <v>630</v>
       </c>
@@ -7780,8 +8239,11 @@
       <c r="I149" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="150" spans="1:9">
+      <c r="J149" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150" s="2" t="s">
         <v>556</v>
       </c>
@@ -7809,8 +8271,11 @@
       <c r="I150" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="151" spans="1:9">
+      <c r="J150" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151" s="2" t="s">
         <v>632</v>
       </c>
@@ -7838,8 +8303,11 @@
       <c r="I151" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="152" spans="1:9">
+      <c r="J151" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152" s="2" t="s">
         <v>640</v>
       </c>
@@ -7867,8 +8335,11 @@
       <c r="I152" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="153" spans="1:9">
+      <c r="J152" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153" s="2" t="s">
         <v>564</v>
       </c>
@@ -7896,8 +8367,11 @@
       <c r="I153" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="154" spans="1:9">
+      <c r="J153" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
       <c r="A154" s="2" t="s">
         <v>635</v>
       </c>
@@ -7925,8 +8399,11 @@
       <c r="I154" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="155" spans="1:9">
+      <c r="J154" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
       <c r="A155" s="2" t="s">
         <v>559</v>
       </c>
@@ -7954,8 +8431,11 @@
       <c r="I155" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="156" spans="1:9">
+      <c r="J155" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
       <c r="A156" s="2" t="s">
         <v>575</v>
       </c>
@@ -7983,8 +8463,11 @@
       <c r="I156" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="157" spans="1:9">
+      <c r="J156" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
       <c r="A157" s="2" t="s">
         <v>577</v>
       </c>
@@ -8012,8 +8495,11 @@
       <c r="I157" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="158" spans="1:9">
+      <c r="J157" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
       <c r="A158" s="2" t="s">
         <v>531</v>
       </c>
@@ -8041,8 +8527,11 @@
       <c r="I158" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="159" spans="1:9">
+      <c r="J158" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
       <c r="A159" s="2" t="s">
         <v>502</v>
       </c>
@@ -8070,8 +8559,11 @@
       <c r="I159" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="160" spans="1:9">
+      <c r="J159" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
       <c r="A160" s="2" t="s">
         <v>504</v>
       </c>
@@ -8099,8 +8591,11 @@
       <c r="I160" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="161" spans="1:9">
+      <c r="J160" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
       <c r="A161" s="2" t="s">
         <v>582</v>
       </c>
@@ -8128,8 +8623,11 @@
       <c r="I161" s="2">
         <v>-31</v>
       </c>
-    </row>
-    <row r="162" spans="1:9">
+      <c r="J161" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162" s="2" t="s">
         <v>625</v>
       </c>
@@ -8157,8 +8655,11 @@
       <c r="I162" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="163" spans="1:9">
+      <c r="J162" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
       <c r="A163" s="2" t="s">
         <v>304</v>
       </c>
@@ -8186,8 +8687,11 @@
       <c r="I163" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="164" spans="1:9">
+      <c r="J163" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10">
       <c r="A164" s="2" t="s">
         <v>561</v>
       </c>
@@ -8215,8 +8719,11 @@
       <c r="I164" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="165" spans="1:9">
+      <c r="J164" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10">
       <c r="A165" s="2" t="s">
         <v>749</v>
       </c>
@@ -8244,8 +8751,11 @@
       <c r="I165" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="166" spans="1:9">
+      <c r="J165" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
       <c r="A166" s="2" t="s">
         <v>794</v>
       </c>
@@ -8273,8 +8783,11 @@
       <c r="I166" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="167" spans="1:9">
+      <c r="J166" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10">
       <c r="A167" s="2" t="s">
         <v>658</v>
       </c>
@@ -8302,8 +8815,11 @@
       <c r="I167" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="168" spans="1:9">
+      <c r="J167" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10">
       <c r="A168" s="2" t="s">
         <v>656</v>
       </c>
@@ -8331,8 +8847,11 @@
       <c r="I168" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="169" spans="1:9">
+      <c r="J168" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10">
       <c r="A169" s="2" t="s">
         <v>659</v>
       </c>
@@ -8360,8 +8879,11 @@
       <c r="I169" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="170" spans="1:9">
+      <c r="J169" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
       <c r="A170" s="2" t="s">
         <v>654</v>
       </c>
@@ -8389,8 +8911,11 @@
       <c r="I170" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="171" spans="1:9">
+      <c r="J170" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
       <c r="A171" s="2" t="s">
         <v>689</v>
       </c>
@@ -8418,8 +8943,11 @@
       <c r="I171" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="172" spans="1:9">
+      <c r="J171" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10">
       <c r="A172" s="2" t="s">
         <v>189</v>
       </c>
@@ -8447,8 +8975,11 @@
       <c r="I172" s="2">
         <v>-17</v>
       </c>
-    </row>
-    <row r="173" spans="1:9">
+      <c r="J172" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10">
       <c r="A173" s="2" t="s">
         <v>698</v>
       </c>
@@ -8476,8 +9007,11 @@
       <c r="I173" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="174" spans="1:9">
+      <c r="J173" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10">
       <c r="A174" s="2" t="s">
         <v>735</v>
       </c>
@@ -8505,8 +9039,11 @@
       <c r="I174" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="175" spans="1:9">
+      <c r="J174" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10">
       <c r="A175" s="2" t="s">
         <v>750</v>
       </c>
@@ -8534,8 +9071,11 @@
       <c r="I175" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="176" spans="1:9">
+      <c r="J175" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10">
       <c r="A176" s="2" t="s">
         <v>751</v>
       </c>
@@ -8563,8 +9103,11 @@
       <c r="I176" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="177" spans="1:9">
+      <c r="J176" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10">
       <c r="A177" s="2" t="s">
         <v>752</v>
       </c>
@@ -8592,8 +9135,11 @@
       <c r="I177" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="178" spans="1:9">
+      <c r="J177" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10">
       <c r="A178" s="2" t="s">
         <v>753</v>
       </c>
@@ -8621,8 +9167,11 @@
       <c r="I178" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="179" spans="1:9">
+      <c r="J178" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10">
       <c r="A179" s="2" t="s">
         <v>754</v>
       </c>
@@ -8650,8 +9199,11 @@
       <c r="I179" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="180" spans="1:9">
+      <c r="J179" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10">
       <c r="A180" s="2" t="s">
         <v>327</v>
       </c>
@@ -8679,8 +9231,11 @@
       <c r="I180" s="2">
         <v>-16</v>
       </c>
-    </row>
-    <row r="181" spans="1:9">
+      <c r="J180" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10">
       <c r="A181" s="2" t="s">
         <v>763</v>
       </c>
@@ -8708,8 +9263,11 @@
       <c r="I181" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="182" spans="1:9">
+      <c r="J181" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10">
       <c r="A182" s="2" t="s">
         <v>799</v>
       </c>
@@ -8737,8 +9295,11 @@
       <c r="I182" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="183" spans="1:9">
+      <c r="J182" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10">
       <c r="A183" s="2" t="s">
         <v>800</v>
       </c>
@@ -8766,8 +9327,11 @@
       <c r="I183" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="184" spans="1:9">
+      <c r="J183" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10">
       <c r="A184" s="2" t="s">
         <v>676</v>
       </c>
@@ -8795,8 +9359,11 @@
       <c r="I184" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="185" spans="1:9">
+      <c r="J184" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10">
       <c r="A185" s="2" t="s">
         <v>757</v>
       </c>
@@ -8824,8 +9391,11 @@
       <c r="I185" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="1:9">
+      <c r="J185" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10">
       <c r="A186" s="2" t="s">
         <v>341</v>
       </c>
@@ -8853,8 +9423,11 @@
       <c r="I186" s="2" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="187" spans="1:9">
+      <c r="J186" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10">
       <c r="A187" s="2" t="s">
         <v>343</v>
       </c>
@@ -8882,8 +9455,11 @@
       <c r="I187" s="2" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="188" spans="1:9">
+      <c r="J187" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10">
       <c r="A188" s="2" t="s">
         <v>346</v>
       </c>
@@ -8911,8 +9487,11 @@
       <c r="I188" s="2" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="189" spans="1:9">
+      <c r="J188" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10">
       <c r="A189" s="2" t="s">
         <v>348</v>
       </c>
@@ -8940,8 +9519,11 @@
       <c r="I189" s="2" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="190" spans="1:9">
+      <c r="J189" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10">
       <c r="A190" s="2" t="s">
         <v>785</v>
       </c>
@@ -8969,8 +9551,11 @@
       <c r="I190" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="191" spans="1:9">
+      <c r="J190" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10">
       <c r="A191" s="2" t="s">
         <v>805</v>
       </c>
@@ -8998,8 +9583,11 @@
       <c r="I191" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="192" spans="1:9">
+      <c r="J191" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10">
       <c r="A192" s="2" t="s">
         <v>806</v>
       </c>
@@ -9027,8 +9615,11 @@
       <c r="I192" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="193" spans="1:9">
+      <c r="J192" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10">
       <c r="A193" s="2" t="s">
         <v>471</v>
       </c>
@@ -9056,8 +9647,11 @@
       <c r="I193" s="2">
         <v>-16</v>
       </c>
-    </row>
-    <row r="194" spans="1:9">
+      <c r="J193" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10">
       <c r="A194" s="2" t="s">
         <v>740</v>
       </c>
@@ -9085,8 +9679,11 @@
       <c r="I194" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="1:9">
+      <c r="J194" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10">
       <c r="A195" s="2" t="s">
         <v>741</v>
       </c>
@@ -9114,8 +9711,11 @@
       <c r="I195" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="196" spans="1:9">
+      <c r="J195" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10">
       <c r="A196" s="2" t="s">
         <v>742</v>
       </c>
@@ -9143,8 +9743,11 @@
       <c r="I196" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="197" spans="1:9">
+      <c r="J196" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10">
       <c r="A197" s="2" t="s">
         <v>682</v>
       </c>
@@ -9172,8 +9775,11 @@
       <c r="I197" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="1:9">
+      <c r="J197" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10">
       <c r="A198" s="2" t="s">
         <v>268</v>
       </c>
@@ -9201,8 +9807,11 @@
       <c r="I198" s="2">
         <v>-16</v>
       </c>
-    </row>
-    <row r="199" spans="1:9">
+      <c r="J198" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10">
       <c r="A199" s="2" t="s">
         <v>814</v>
       </c>
@@ -9230,8 +9839,11 @@
       <c r="I199" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="200" spans="1:9">
+      <c r="J199" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10">
       <c r="A200" s="2" t="s">
         <v>496</v>
       </c>
@@ -9259,8 +9871,11 @@
       <c r="I200" s="2">
         <v>-30</v>
       </c>
-    </row>
-    <row r="201" spans="1:9">
+      <c r="J200" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10">
       <c r="A201" s="2" t="s">
         <v>566</v>
       </c>
@@ -9288,8 +9903,11 @@
       <c r="I201" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="202" spans="1:9">
+      <c r="J201" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10">
       <c r="A202" s="2" t="s">
         <v>568</v>
       </c>
@@ -9317,8 +9935,11 @@
       <c r="I202" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="203" spans="1:9">
+      <c r="J202" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10">
       <c r="A203" s="2" t="s">
         <v>745</v>
       </c>
@@ -9346,8 +9967,11 @@
       <c r="I203" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="204" spans="1:9">
+      <c r="J203" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10">
       <c r="A204" s="2" t="s">
         <v>746</v>
       </c>
@@ -9375,8 +9999,11 @@
       <c r="I204" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="205" spans="1:9">
+      <c r="J204" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10">
       <c r="A205" s="2" t="s">
         <v>747</v>
       </c>
@@ -9404,8 +10031,11 @@
       <c r="I205" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="206" spans="1:9">
+      <c r="J205" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10">
       <c r="A206" s="2" t="s">
         <v>748</v>
       </c>
@@ -9433,8 +10063,11 @@
       <c r="I206" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="1:9">
+      <c r="J206" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10">
       <c r="A207" s="2" t="s">
         <v>306</v>
       </c>
@@ -9462,8 +10095,11 @@
       <c r="I207" s="2">
         <v>-20</v>
       </c>
-    </row>
-    <row r="208" spans="1:9">
+      <c r="J207" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10">
       <c r="A208" s="2" t="s">
         <v>313</v>
       </c>
@@ -9491,8 +10127,11 @@
       <c r="I208" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="209" spans="1:9">
+      <c r="J208" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10">
       <c r="A209" s="2" t="s">
         <v>510</v>
       </c>
@@ -9520,8 +10159,11 @@
       <c r="I209" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="210" spans="1:9">
+      <c r="J209" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10">
       <c r="A210" s="2" t="s">
         <v>517</v>
       </c>
@@ -9549,8 +10191,11 @@
       <c r="I210" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="211" spans="1:9">
+      <c r="J210" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10">
       <c r="A211" s="2" t="s">
         <v>662</v>
       </c>
@@ -9578,8 +10223,11 @@
       <c r="I211" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="212" spans="1:9">
+      <c r="J211" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10">
       <c r="A212" s="2" t="s">
         <v>665</v>
       </c>
@@ -9607,8 +10255,11 @@
       <c r="I212" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="213" spans="1:9">
+      <c r="J212" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10">
       <c r="A213" s="2" t="s">
         <v>666</v>
       </c>
@@ -9636,8 +10287,11 @@
       <c r="I213" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="214" spans="1:9">
+      <c r="J213" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10">
       <c r="A214" s="2" t="s">
         <v>55</v>
       </c>
@@ -9665,8 +10319,11 @@
       <c r="I214" s="2" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="215" spans="1:9">
+      <c r="J214" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10">
       <c r="A215" s="2" t="s">
         <v>523</v>
       </c>
@@ -9694,8 +10351,11 @@
       <c r="I215" s="2" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="216" spans="1:9">
+      <c r="J215" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10">
       <c r="A216" s="2" t="s">
         <v>664</v>
       </c>
@@ -9723,8 +10383,11 @@
       <c r="I216" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="217" spans="1:9">
+      <c r="J216" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10">
       <c r="A217" s="2" t="s">
         <v>50</v>
       </c>
@@ -9752,8 +10415,11 @@
       <c r="I217" s="2">
         <v>-2</v>
       </c>
-    </row>
-    <row r="218" spans="1:9">
+      <c r="J217" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10">
       <c r="A218" s="2" t="s">
         <v>53</v>
       </c>
@@ -9781,8 +10447,11 @@
       <c r="I218" s="2" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="219" spans="1:9">
+      <c r="J218" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10">
       <c r="A219" s="2" t="s">
         <v>545</v>
       </c>
@@ -9810,8 +10479,11 @@
       <c r="I219" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="220" spans="1:9">
+      <c r="J219" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10">
       <c r="A220" s="2" t="s">
         <v>547</v>
       </c>
@@ -9839,8 +10511,11 @@
       <c r="I220" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="221" spans="1:9">
+      <c r="J220" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10">
       <c r="A221" s="2" t="s">
         <v>167</v>
       </c>
@@ -9868,8 +10543,11 @@
       <c r="I221" s="2" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="222" spans="1:9">
+      <c r="J221" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10">
       <c r="A222" s="2" t="s">
         <v>715</v>
       </c>
@@ -9897,8 +10575,11 @@
       <c r="I222" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="223" spans="1:9">
+      <c r="J222" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10">
       <c r="A223" s="2" t="s">
         <v>395</v>
       </c>
@@ -9926,8 +10607,11 @@
       <c r="I223" s="2" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="224" spans="1:9">
+      <c r="J223" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10">
       <c r="A224" s="2" t="s">
         <v>406</v>
       </c>
@@ -9955,8 +10639,11 @@
       <c r="I224" s="2">
         <v>-24</v>
       </c>
-    </row>
-    <row r="225" spans="1:9">
+      <c r="J224" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10">
       <c r="A225" s="2" t="s">
         <v>408</v>
       </c>
@@ -9984,8 +10671,11 @@
       <c r="I225" s="2">
         <v>-24</v>
       </c>
-    </row>
-    <row r="226" spans="1:9">
+      <c r="J225" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10">
       <c r="A226" s="2" t="s">
         <v>410</v>
       </c>
@@ -10013,8 +10703,11 @@
       <c r="I226" s="2">
         <v>-24</v>
       </c>
-    </row>
-    <row r="227" spans="1:9">
+      <c r="J226" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10">
       <c r="A227" s="2" t="s">
         <v>412</v>
       </c>
@@ -10042,8 +10735,11 @@
       <c r="I227" s="2">
         <v>-24</v>
       </c>
-    </row>
-    <row r="228" spans="1:9">
+      <c r="J227" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10">
       <c r="A228" s="2" t="s">
         <v>241</v>
       </c>
@@ -10071,8 +10767,11 @@
       <c r="I228" s="2">
         <v>-16</v>
       </c>
-    </row>
-    <row r="229" spans="1:9">
+      <c r="J228" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10">
       <c r="A229" s="2" t="s">
         <v>719</v>
       </c>
@@ -10100,8 +10799,11 @@
       <c r="I229" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="230" spans="1:9">
+      <c r="J229" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10">
       <c r="A230" s="2" t="s">
         <v>397</v>
       </c>
@@ -10129,8 +10831,11 @@
       <c r="I230" s="2" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="231" spans="1:9">
+      <c r="J230" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10">
       <c r="A231" s="2" t="s">
         <v>706</v>
       </c>
@@ -10158,8 +10863,11 @@
       <c r="I231" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="232" spans="1:9">
+      <c r="J231" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10">
       <c r="A232" s="2" t="s">
         <v>402</v>
       </c>
@@ -10187,8 +10895,11 @@
       <c r="I232" s="2" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="233" spans="1:9">
+      <c r="J232" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10">
       <c r="A233" s="2" t="s">
         <v>700</v>
       </c>
@@ -10216,8 +10927,11 @@
       <c r="I233" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="234" spans="1:9">
+      <c r="J233" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10">
       <c r="A234" s="2" t="s">
         <v>701</v>
       </c>
@@ -10245,8 +10959,11 @@
       <c r="I234" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="235" spans="1:9">
+      <c r="J234" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10">
       <c r="A235" s="2" t="s">
         <v>702</v>
       </c>
@@ -10274,8 +10991,11 @@
       <c r="I235" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="236" spans="1:9">
+      <c r="J235" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10">
       <c r="A236" s="2" t="s">
         <v>703</v>
       </c>
@@ -10303,8 +11023,11 @@
       <c r="I236" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="237" spans="1:9">
+      <c r="J236" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10">
       <c r="A237" s="2" t="s">
         <v>773</v>
       </c>
@@ -10332,8 +11055,11 @@
       <c r="I237" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="238" spans="1:9">
+      <c r="J237" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10">
       <c r="A238" s="2" t="s">
         <v>774</v>
       </c>
@@ -10361,8 +11087,11 @@
       <c r="I238" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="239" spans="1:9">
+      <c r="J238" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10">
       <c r="A239" s="2" t="s">
         <v>775</v>
       </c>
@@ -10390,8 +11119,11 @@
       <c r="I239" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="240" spans="1:9">
+      <c r="J239" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10">
       <c r="A240" s="2" t="s">
         <v>777</v>
       </c>
@@ -10419,8 +11151,11 @@
       <c r="I240" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="241" spans="1:9">
+      <c r="J240" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10">
       <c r="A241" s="2" t="s">
         <v>779</v>
       </c>
@@ -10448,8 +11183,11 @@
       <c r="I241" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="242" spans="1:9">
+      <c r="J241" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10">
       <c r="A242" s="2" t="s">
         <v>782</v>
       </c>
@@ -10477,8 +11215,11 @@
       <c r="I242" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="243" spans="1:9">
+      <c r="J242" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10">
       <c r="A243" s="2" t="s">
         <v>783</v>
       </c>
@@ -10506,8 +11247,11 @@
       <c r="I243" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="244" spans="1:9">
+      <c r="J243" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10">
       <c r="A244" s="2" t="s">
         <v>784</v>
       </c>
@@ -10535,8 +11279,11 @@
       <c r="I244" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="245" spans="1:9">
+      <c r="J244" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10">
       <c r="A245" s="2" t="s">
         <v>707</v>
       </c>
@@ -10564,8 +11311,11 @@
       <c r="I245" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="246" spans="1:9">
+      <c r="J245" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10">
       <c r="A246" s="2" t="s">
         <v>708</v>
       </c>
@@ -10593,8 +11343,11 @@
       <c r="I246" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="247" spans="1:9">
+      <c r="J246" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10">
       <c r="A247" s="2" t="s">
         <v>709</v>
       </c>
@@ -10622,8 +11375,11 @@
       <c r="I247" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="248" spans="1:9">
+      <c r="J247" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10">
       <c r="A248" s="2" t="s">
         <v>710</v>
       </c>
@@ -10651,8 +11407,11 @@
       <c r="I248" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="249" spans="1:9">
+      <c r="J248" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10">
       <c r="A249" s="2" t="s">
         <v>711</v>
       </c>
@@ -10680,8 +11439,11 @@
       <c r="I249" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="250" spans="1:9">
+      <c r="J249" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10">
       <c r="A250" s="2" t="s">
         <v>778</v>
       </c>
@@ -10709,8 +11471,11 @@
       <c r="I250" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="251" spans="1:9">
+      <c r="J250" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10">
       <c r="A251" s="2" t="s">
         <v>781</v>
       </c>
@@ -10738,8 +11503,11 @@
       <c r="I251" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="252" spans="1:9">
+      <c r="J251" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10">
       <c r="A252" s="2" t="s">
         <v>793</v>
       </c>
@@ -10767,8 +11535,11 @@
       <c r="I252" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="253" spans="1:9">
+      <c r="J252" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10">
       <c r="A253" s="2" t="s">
         <v>798</v>
       </c>
@@ -10796,8 +11567,11 @@
       <c r="I253" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="254" spans="1:9">
+      <c r="J253" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10">
       <c r="A254" s="2" t="s">
         <v>714</v>
       </c>
@@ -10825,8 +11599,11 @@
       <c r="I254" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="255" spans="1:9">
+      <c r="J254" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10">
       <c r="A255" s="2" t="s">
         <v>716</v>
       </c>
@@ -10854,8 +11631,11 @@
       <c r="I255" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="256" spans="1:9">
+      <c r="J255" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10">
       <c r="A256" s="2" t="s">
         <v>717</v>
       </c>
@@ -10883,8 +11663,11 @@
       <c r="I256" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="257" spans="1:9">
+      <c r="J256" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10">
       <c r="A257" s="2" t="s">
         <v>718</v>
       </c>
@@ -10912,8 +11695,11 @@
       <c r="I257" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="258" spans="1:9">
+      <c r="J257" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10">
       <c r="A258" s="2" t="s">
         <v>720</v>
       </c>
@@ -10941,8 +11727,11 @@
       <c r="I258" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="259" spans="1:9">
+      <c r="J258" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10">
       <c r="A259" s="2" t="s">
         <v>721</v>
       </c>
@@ -10970,8 +11759,11 @@
       <c r="I259" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="260" spans="1:9">
+      <c r="J259" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10">
       <c r="A260" s="2" t="s">
         <v>722</v>
       </c>
@@ -10999,8 +11791,11 @@
       <c r="I260" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="261" spans="1:9">
+      <c r="J260" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10">
       <c r="A261" s="2" t="s">
         <v>723</v>
       </c>
@@ -11028,8 +11823,11 @@
       <c r="I261" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="262" spans="1:9">
+      <c r="J261" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10">
       <c r="A262" s="2" t="s">
         <v>726</v>
       </c>
@@ -11057,8 +11855,11 @@
       <c r="I262" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="263" spans="1:9">
+      <c r="J262" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10">
       <c r="A263" s="2" t="s">
         <v>727</v>
       </c>
@@ -11086,8 +11887,11 @@
       <c r="I263" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="264" spans="1:9">
+      <c r="J263" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10">
       <c r="A264" s="2" t="s">
         <v>728</v>
       </c>
@@ -11115,8 +11919,11 @@
       <c r="I264" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="265" spans="1:9">
+      <c r="J264" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10">
       <c r="A265" s="2" t="s">
         <v>729</v>
       </c>
@@ -11144,8 +11951,11 @@
       <c r="I265" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="266" spans="1:9">
+      <c r="J265" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10">
       <c r="A266" s="2" t="s">
         <v>730</v>
       </c>
@@ -11173,8 +11983,11 @@
       <c r="I266" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="267" spans="1:9">
+      <c r="J266" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10">
       <c r="A267" s="2" t="s">
         <v>731</v>
       </c>
@@ -11202,8 +12015,11 @@
       <c r="I267" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="268" spans="1:9">
+      <c r="J267" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10">
       <c r="A268" s="2" t="s">
         <v>764</v>
       </c>
@@ -11231,8 +12047,11 @@
       <c r="I268" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="269" spans="1:9">
+      <c r="J268" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10">
       <c r="A269" s="2" t="s">
         <v>765</v>
       </c>
@@ -11260,8 +12079,11 @@
       <c r="I269" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="270" spans="1:9">
+      <c r="J269" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10">
       <c r="A270" s="2" t="s">
         <v>786</v>
       </c>
@@ -11289,8 +12111,11 @@
       <c r="I270" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="271" spans="1:9">
+      <c r="J270" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10">
       <c r="A271" s="2" t="s">
         <v>787</v>
       </c>
@@ -11318,8 +12143,11 @@
       <c r="I271" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="272" spans="1:9">
+      <c r="J271" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10">
       <c r="A272" s="2" t="s">
         <v>788</v>
       </c>
@@ -11347,8 +12175,11 @@
       <c r="I272" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="273" spans="1:9">
+      <c r="J272" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10">
       <c r="A273" s="2" t="s">
         <v>789</v>
       </c>
@@ -11376,8 +12207,11 @@
       <c r="I273" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="274" spans="1:9">
+      <c r="J273" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10">
       <c r="A274" s="2" t="s">
         <v>790</v>
       </c>
@@ -11405,8 +12239,11 @@
       <c r="I274" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="275" spans="1:9">
+      <c r="J274" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10">
       <c r="A275" s="2" t="s">
         <v>786</v>
       </c>
@@ -11434,8 +12271,11 @@
       <c r="I275" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="276" spans="1:9">
+      <c r="J275" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10">
       <c r="A276" s="2" t="s">
         <v>813</v>
       </c>
@@ -11463,8 +12303,11 @@
       <c r="I276" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="277" spans="1:9">
+      <c r="J276" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10">
       <c r="A277" s="2" t="s">
         <v>724</v>
       </c>
@@ -11492,8 +12335,11 @@
       <c r="I277" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="278" spans="1:9">
+      <c r="J277" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10">
       <c r="A278" s="2" t="s">
         <v>725</v>
       </c>
@@ -11521,8 +12367,11 @@
       <c r="I278" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="279" spans="1:9">
+      <c r="J278" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10">
       <c r="A279" s="2" t="s">
         <v>807</v>
       </c>
@@ -11550,8 +12399,11 @@
       <c r="I279" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="280" spans="1:9">
+      <c r="J279" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10">
       <c r="A280" s="2" t="s">
         <v>808</v>
       </c>
@@ -11579,8 +12431,11 @@
       <c r="I280" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="281" spans="1:9">
+      <c r="J280" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10">
       <c r="A281" s="2" t="s">
         <v>809</v>
       </c>
@@ -11608,8 +12463,11 @@
       <c r="I281" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="282" spans="1:9">
+      <c r="J281" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10">
       <c r="A282" s="2" t="s">
         <v>810</v>
       </c>
@@ -11637,8 +12495,11 @@
       <c r="I282" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="283" spans="1:9">
+      <c r="J282" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10">
       <c r="A283" s="2" t="s">
         <v>811</v>
       </c>
@@ -11666,8 +12527,11 @@
       <c r="I283" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="284" spans="1:9">
+      <c r="J283" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10">
       <c r="A284" s="2" t="s">
         <v>812</v>
       </c>
@@ -11695,8 +12559,11 @@
       <c r="I284" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="285" spans="1:9">
+      <c r="J284" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10">
       <c r="A285" s="2" t="s">
         <v>683</v>
       </c>
@@ -11724,8 +12591,11 @@
       <c r="I285" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="286" spans="1:9">
+      <c r="J285" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10">
       <c r="A286" s="2" t="s">
         <v>684</v>
       </c>
@@ -11753,8 +12623,11 @@
       <c r="I286" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="287" spans="1:9">
+      <c r="J286" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10">
       <c r="A287" s="2" t="s">
         <v>685</v>
       </c>
@@ -11782,8 +12655,11 @@
       <c r="I287" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="288" spans="1:9">
+      <c r="J287" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10">
       <c r="A288" s="2" t="s">
         <v>686</v>
       </c>
@@ -11811,8 +12687,11 @@
       <c r="I288" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="289" spans="1:9">
+      <c r="J288" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10">
       <c r="A289" s="2" t="s">
         <v>687</v>
       </c>
@@ -11840,8 +12719,11 @@
       <c r="I289" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="290" spans="1:9">
+      <c r="J289" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10">
       <c r="A290" s="2" t="s">
         <v>688</v>
       </c>
@@ -11869,8 +12751,11 @@
       <c r="I290" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="291" spans="1:9">
+      <c r="J290" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10">
       <c r="A291" s="2" t="s">
         <v>184</v>
       </c>
@@ -11898,8 +12783,11 @@
       <c r="I291" s="2">
         <v>-16</v>
       </c>
-    </row>
-    <row r="292" spans="1:9">
+      <c r="J291" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10">
       <c r="A292" s="2" t="s">
         <v>690</v>
       </c>
@@ -11927,8 +12815,11 @@
       <c r="I292" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="293" spans="1:9">
+      <c r="J292" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10">
       <c r="A293" s="2" t="s">
         <v>691</v>
       </c>
@@ -11956,8 +12847,11 @@
       <c r="I293" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="294" spans="1:9">
+      <c r="J293" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10">
       <c r="A294" s="2" t="s">
         <v>771</v>
       </c>
@@ -11985,8 +12879,11 @@
       <c r="I294" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="295" spans="1:9">
+      <c r="J294" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10">
       <c r="A295" s="2" t="s">
         <v>772</v>
       </c>
@@ -12014,8 +12911,11 @@
       <c r="I295" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="296" spans="1:9">
+      <c r="J295" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10">
       <c r="A296" s="2" t="s">
         <v>776</v>
       </c>
@@ -12043,8 +12943,11 @@
       <c r="I296" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="297" spans="1:9">
+      <c r="J296" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10">
       <c r="A297" s="2" t="s">
         <v>780</v>
       </c>
@@ -12072,8 +12975,11 @@
       <c r="I297" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="298" spans="1:9">
+      <c r="J297" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10">
       <c r="A298" s="2" t="s">
         <v>404</v>
       </c>
@@ -12101,8 +13007,11 @@
       <c r="I298" s="2" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="299" spans="1:9">
+      <c r="J298" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10">
       <c r="A299" s="2" t="s">
         <v>335</v>
       </c>
@@ -12130,8 +13039,11 @@
       <c r="I299" s="2">
         <v>-21</v>
       </c>
-    </row>
-    <row r="300" spans="1:9">
+      <c r="J299" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10">
       <c r="A300" s="2" t="s">
         <v>692</v>
       </c>
@@ -12159,8 +13071,11 @@
       <c r="I300" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="301" spans="1:9">
+      <c r="J300" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10">
       <c r="A301" s="2" t="s">
         <v>693</v>
       </c>
@@ -12188,8 +13103,11 @@
       <c r="I301" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="302" spans="1:9">
+      <c r="J301" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10">
       <c r="A302" s="2" t="s">
         <v>694</v>
       </c>
@@ -12217,8 +13135,11 @@
       <c r="I302" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="303" spans="1:9">
+      <c r="J302" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10">
       <c r="A303" s="2" t="s">
         <v>695</v>
       </c>
@@ -12246,8 +13167,11 @@
       <c r="I303" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="304" spans="1:9">
+      <c r="J303" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10">
       <c r="A304" s="2" t="s">
         <v>699</v>
       </c>
@@ -12275,8 +13199,11 @@
       <c r="I304" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="305" spans="1:9">
+      <c r="J304" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10">
       <c r="A305" s="2" t="s">
         <v>795</v>
       </c>
@@ -12304,8 +13231,11 @@
       <c r="I305" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="306" spans="1:9">
+      <c r="J305" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10">
       <c r="A306" s="2" t="s">
         <v>796</v>
       </c>
@@ -12333,8 +13263,11 @@
       <c r="I306" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="307" spans="1:9">
+      <c r="J306" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10">
       <c r="A307" s="2" t="s">
         <v>797</v>
       </c>
@@ -12362,8 +13295,11 @@
       <c r="I307" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="308" spans="1:9">
+      <c r="J307" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10">
       <c r="A308" s="2" t="s">
         <v>659</v>
       </c>
@@ -12391,8 +13327,11 @@
       <c r="I308" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="309" spans="1:9">
+      <c r="J308" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10">
       <c r="A309" s="2" t="s">
         <v>712</v>
       </c>
@@ -12420,8 +13359,11 @@
       <c r="I309" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="310" spans="1:9">
+      <c r="J309" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10">
       <c r="A310" s="2" t="s">
         <v>758</v>
       </c>
@@ -12449,8 +13391,11 @@
       <c r="I310" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="311" spans="1:9">
+      <c r="J310" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10">
       <c r="A311" s="2" t="s">
         <v>759</v>
       </c>
@@ -12478,8 +13423,11 @@
       <c r="I311" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="312" spans="1:9">
+      <c r="J311" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10">
       <c r="A312" s="2" t="s">
         <v>457</v>
       </c>
@@ -12507,8 +13455,11 @@
       <c r="I312" s="2">
         <v>-26</v>
       </c>
-    </row>
-    <row r="313" spans="1:9">
+      <c r="J312" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10">
       <c r="A313" s="2" t="s">
         <v>459</v>
       </c>
@@ -12536,8 +13487,11 @@
       <c r="I313" s="2">
         <v>-16</v>
       </c>
-    </row>
-    <row r="314" spans="1:9">
+      <c r="J313" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10">
       <c r="A314" s="2" t="s">
         <v>310</v>
       </c>
@@ -12565,8 +13519,11 @@
       <c r="I314" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="315" spans="1:9">
+      <c r="J314" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10">
       <c r="A315" s="2" t="s">
         <v>315</v>
       </c>
@@ -12594,8 +13551,11 @@
       <c r="I315" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="316" spans="1:9">
+      <c r="J315" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10">
       <c r="A316" s="2" t="s">
         <v>74</v>
       </c>
@@ -12623,8 +13583,11 @@
       <c r="I316" s="2">
         <v>-3</v>
       </c>
-    </row>
-    <row r="317" spans="1:9">
+      <c r="J316" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10">
       <c r="A317" s="2" t="s">
         <v>579</v>
       </c>
@@ -12652,8 +13615,11 @@
       <c r="I317" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="318" spans="1:9">
+      <c r="J317" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10">
       <c r="A318" s="2" t="s">
         <v>513</v>
       </c>
@@ -12681,8 +13647,11 @@
       <c r="I318" s="2">
         <v>-19</v>
       </c>
-    </row>
-    <row r="319" spans="1:9">
+      <c r="J318" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10">
       <c r="A319" s="2" t="s">
         <v>515</v>
       </c>
@@ -12709,6 +13678,9 @@
       </c>
       <c r="I319" s="2">
         <v>-19</v>
+      </c>
+      <c r="J319" s="2" t="s">
+        <v>890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>